<commit_message>
Added all leaderboard functionality
</commit_message>
<xml_diff>
--- a/Assets/Leaderboard.xlsx
+++ b/Assets/Leaderboard.xlsx
@@ -1,77 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdmea\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A4FF2D5-A4D2-464E-9EA2-908B34484FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{6BA06A3D-AFD9-4A57-8767-CCBA0A5B4D1F}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5115" yWindow="4185" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lance </t>
-  </si>
-  <si>
-    <t>Connor</t>
-  </si>
-  <si>
-    <t>Phillip</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -90,21 +52,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -424,73 +445,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7D0700-4947-4773-BC9A-B830135609C0}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Phillip</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D1" t="n">
+        <v>0.167</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Jack</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
         <v>5</v>
       </c>
-      <c r="C1">
+      <c r="D2" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lance </t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Lance</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>4</v>
       </c>
-      <c r="D1">
-        <v>1.25</v>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Connor</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="D5" t="n">
         <v>3</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed all debugging statments
</commit_message>
<xml_diff>
--- a/Assets/Leaderboard.xlsx
+++ b/Assets/Leaderboard.xlsx
@@ -461,65 +461,65 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Lance</t>
+          <t>Jack</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D1" t="n">
-        <v>4</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Connor</t>
+          <t>Lance</t>
         </is>
       </c>
       <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
         <v>3</v>
       </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>1.333</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jack</t>
+          <t xml:space="preserve">Lance </t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lance </t>
+          <t>Connor</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>3</v>
       </c>
       <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
         <v>3</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="5">

</xml_diff>